<commit_message>
Add controller for demo
</commit_message>
<xml_diff>
--- a/cherry_project/Resources/Sogeti.xlsx
+++ b/cherry_project/Resources/Sogeti.xlsx
@@ -60,9 +60,6 @@
     <t>question_behave</t>
   </si>
   <si>
-    <t xml:space="preserve"> Digital, Testing, Secutrité, et Infrastructures</t>
-  </si>
-  <si>
     <t>Sogeti se distingue dans 4 domaines</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>Slide</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Digital, Testing, Securité, et Infrastructures</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -450,13 +450,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -494,10 +494,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -508,7 +508,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>

</xml_diff>